<commit_message>
Completed most of processing code
</commit_message>
<xml_diff>
--- a/test/calculating_readm_for_testing.xlsx
+++ b/test/calculating_readm_for_testing.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="formulae" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="112">
   <si>
     <t>f/hig437a/dm/comorb2</t>
   </si>
@@ -117,12 +117,6 @@
     <t>hig=208a</t>
   </si>
   <si>
-    <t>pneu-hig138</t>
-  </si>
-  <si>
-    <t>gi-hig288</t>
-  </si>
-  <si>
     <t>fiscal_qtr=1</t>
   </si>
   <si>
@@ -261,32 +255,134 @@
     <t>m/hig194b/age62/fiscal_qtr4/prevadm3/com2/2015</t>
   </si>
   <si>
-    <t>hig285(cirrhosis)</t>
-  </si>
-  <si>
-    <t>hig257(gi sign)</t>
-  </si>
-  <si>
-    <t>hig255(obstruc)</t>
-  </si>
-  <si>
-    <t>hig254(hemmor)</t>
-  </si>
-  <si>
-    <t>hig202(arrhyhmia wo cardio angio)</t>
+    <t>m/hig288(billiar)/qtr4/prevadm3/com2/2015</t>
+  </si>
+  <si>
+    <t>hig=257</t>
+  </si>
+  <si>
+    <t>hig=285</t>
+  </si>
+  <si>
+    <t>hig=255</t>
+  </si>
+  <si>
+    <t>hig=254</t>
+  </si>
+  <si>
+    <t>m/hig288/age62/qtr4/prevadm3/com2/2015</t>
+  </si>
+  <si>
+    <t>f/hig288/age86/qtr4/prevadm3/com2/2015</t>
+  </si>
+  <si>
+    <t>m/hig288/age86/qtr4/prevadm0/com2/2015</t>
+  </si>
+  <si>
+    <t>m/hig288/age86/qtr4/prevadm3/com0/2015</t>
+  </si>
+  <si>
+    <t>m/hig288/age86/qtr4/prevadm3/com2/2014</t>
+  </si>
+  <si>
+    <t>m/hig288/age86/qtr1/prevadm3/com2/2015</t>
+  </si>
+  <si>
+    <t>m/hig257(gisign)/age86/qtr4/prevadm3/com2/2015</t>
+  </si>
+  <si>
+    <t>m/hig285(cirrhosis)/qtr4/prevadm3/com2/2015</t>
+  </si>
+  <si>
+    <t>m/hig255(obstruc)/qtr4/prevadm3/com2/2015</t>
+  </si>
+  <si>
+    <t>m/hig254(hemmor)/qtr4/prevadm3/com2/2015</t>
+  </si>
+  <si>
+    <t>m/hig202/age86/qtr4/prevadm3/com2/2015</t>
+  </si>
+  <si>
+    <t>m/hig208b/qtr4/prevadm3/com2/2015</t>
+  </si>
+  <si>
+    <t>m/hig208b/age62/qtr4/prevadm3/com2/2015</t>
+  </si>
+  <si>
+    <t>f/hig208b/age86/qtr4/prevadm3/com2/2015</t>
+  </si>
+  <si>
+    <t>m/hig208b/age86/qtr4/prevadm0/com2/2015</t>
+  </si>
+  <si>
+    <t>m/hig208b/age86/qtr4/prevadm3/com0/2015</t>
+  </si>
+  <si>
+    <t>m/hig208b/age86/qtr4/prevadm3/com2/2014</t>
+  </si>
+  <si>
+    <t>m/hig208b/age86/qtr1/prevadm3/com2/2015</t>
+  </si>
+  <si>
+    <t>hig=202</t>
+  </si>
+  <si>
+    <t>m/hig139d/qtr4/prevadm3/com2/2015</t>
+  </si>
+  <si>
+    <t>m/hig139d/age62/qtr4/prevadm3/com2/2015</t>
+  </si>
+  <si>
+    <t>f/hig139d/age86/qtr4/prevadm3/com2/2015</t>
+  </si>
+  <si>
+    <t>m/hig139d/age86/qtr4/prevadm0/com2/2015</t>
+  </si>
+  <si>
+    <t>m/hig139d/age86/qtr4/prevadm3/com0/2015</t>
+  </si>
+  <si>
+    <t>m/hig139d/age86/qtr4/prevadm3/com2/2014</t>
+  </si>
+  <si>
+    <t>m/hig139d/age86/qtr1/prevadm3/com2/2015</t>
+  </si>
+  <si>
+    <t>m/hig139c/age86/qtr4/prevadm3/com2/2015</t>
+  </si>
+  <si>
+    <t>hig=139c</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -341,12 +437,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -649,10 +748,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P115"/>
+  <dimension ref="A1:R104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A87" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A88" sqref="A88"/>
+    <sheetView topLeftCell="L85" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O98" sqref="O98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="36.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -662,7 +761,7 @@
     <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="19.42578125" bestFit="1" customWidth="1"/>
@@ -672,7 +771,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -857,7 +956,7 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -1046,7 +1145,7 @@
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
@@ -1075,7 +1174,7 @@
         <v>29</v>
       </c>
       <c r="J22" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="K22" t="s">
         <v>25</v>
@@ -1141,7 +1240,7 @@
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B24" s="2">
         <v>10.478199999999999</v>
@@ -1179,7 +1278,7 @@
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B25" s="2">
         <v>10.478199999999999</v>
@@ -1377,940 +1476,1944 @@
         <v>6.4581864317878837E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>4</v>
+      </c>
+      <c r="C33" t="s">
+        <v>6</v>
+      </c>
+      <c r="D33" t="s">
+        <v>7</v>
+      </c>
+      <c r="E33" t="s">
+        <v>8</v>
+      </c>
+      <c r="F33" t="s">
+        <v>33</v>
+      </c>
+      <c r="G33" t="s">
+        <v>29</v>
+      </c>
+      <c r="H33" t="s">
+        <v>34</v>
+      </c>
+      <c r="I33" t="s">
+        <v>26</v>
+      </c>
+      <c r="J33" t="s">
+        <v>53</v>
+      </c>
+      <c r="K33" t="s">
+        <v>11</v>
+      </c>
+      <c r="L33" t="s">
+        <v>52</v>
+      </c>
+      <c r="M33" t="s">
+        <v>12</v>
+      </c>
+      <c r="N33" t="s">
+        <v>13</v>
+      </c>
+      <c r="O33" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>55</v>
+      </c>
+      <c r="B34" s="3">
+        <v>2.7008999999999999</v>
+      </c>
+      <c r="F34" s="3"/>
+      <c r="G34">
+        <f>0.0123*18</f>
+        <v>0.22140000000000001</v>
+      </c>
+      <c r="I34" s="3"/>
+      <c r="L34" s="3">
+        <f>2015*-0.00177</f>
+        <v>-3.5665500000000003</v>
+      </c>
+      <c r="M34">
+        <f>SUM(B34:L34)</f>
+        <v>-0.64425000000000043</v>
+      </c>
+      <c r="N34">
+        <f>EXP(M34)</f>
+        <v>0.52505618661140985</v>
+      </c>
+      <c r="O34">
+        <f>N34/(N34+1)</f>
+        <v>0.3442864539817746</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>54</v>
+      </c>
+      <c r="B35" s="3">
+        <v>2.7008999999999999</v>
+      </c>
+      <c r="C35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="H35">
+        <f>0.0123*13</f>
+        <v>0.15990000000000001</v>
+      </c>
+      <c r="I35" s="3"/>
+      <c r="K35" s="3"/>
+      <c r="L35" s="3">
+        <f>2015*-0.00177</f>
+        <v>-3.5665500000000003</v>
+      </c>
+      <c r="M35">
+        <f>SUM(B35:L35)</f>
+        <v>-0.70575000000000054</v>
+      </c>
+      <c r="N35">
+        <f>EXP(M35)</f>
+        <v>0.49373813175875031</v>
+      </c>
+      <c r="O35">
+        <f>N35/(N35+1)</f>
+        <v>0.33053861400553214</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>56</v>
+      </c>
+      <c r="B36" s="3">
+        <v>2.7008999999999999</v>
+      </c>
+      <c r="C36" s="3">
+        <v>-6.4000000000000001E-2</v>
+      </c>
+      <c r="D36" s="3"/>
+      <c r="G36">
+        <f>0.0123*18</f>
+        <v>0.22140000000000001</v>
+      </c>
+      <c r="L36" s="3">
+        <f>2015*-0.00177</f>
+        <v>-3.5665500000000003</v>
+      </c>
+      <c r="M36">
+        <f>SUM(B36:L36)</f>
+        <v>-0.70825000000000049</v>
+      </c>
+      <c r="N36">
+        <f>EXP(M36)</f>
+        <v>0.49250532807604203</v>
+      </c>
+      <c r="O36">
+        <f>N36/(N36+1)</f>
+        <v>0.32998564146562914</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>57</v>
+      </c>
+      <c r="B37" s="3">
+        <v>2.7008999999999999</v>
+      </c>
+      <c r="D37" s="3">
+        <v>-0.13669999999999999</v>
+      </c>
+      <c r="G37">
+        <f>0.0123*18</f>
+        <v>0.22140000000000001</v>
+      </c>
+      <c r="L37" s="3">
+        <f>2015*-0.00177</f>
+        <v>-3.5665500000000003</v>
+      </c>
+      <c r="M37">
+        <f>SUM(B37:L37)</f>
+        <v>-0.78095000000000026</v>
+      </c>
+      <c r="N37">
+        <f>EXP(M37)</f>
+        <v>0.45797073238470731</v>
+      </c>
+      <c r="O37">
+        <f>N37/(N37+1)</f>
+        <v>0.31411517543677614</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>4</v>
+      </c>
+      <c r="C43" t="s">
+        <v>32</v>
+      </c>
+      <c r="D43" t="s">
+        <v>6</v>
+      </c>
+      <c r="E43" t="s">
+        <v>7</v>
+      </c>
+      <c r="F43" t="s">
+        <v>8</v>
+      </c>
+      <c r="G43" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>34</v>
+      <c r="H43" t="s">
+        <v>10</v>
+      </c>
+      <c r="I43" t="s">
+        <v>26</v>
+      </c>
+      <c r="J43" t="s">
+        <v>11</v>
+      </c>
+      <c r="K43" t="s">
+        <v>12</v>
+      </c>
+      <c r="L43" t="s">
+        <v>13</v>
+      </c>
+      <c r="M43" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>31</v>
+      </c>
+      <c r="B44" s="2">
+        <v>1.3971</v>
+      </c>
+      <c r="C44" s="2">
+        <v>-8.6199999999999999E-2</v>
+      </c>
+      <c r="D44" s="2">
+        <v>-9.1499999999999998E-2</v>
+      </c>
+      <c r="E44" s="2">
+        <v>-0.68579999999999997</v>
+      </c>
+      <c r="G44" s="2">
+        <v>-8.2699999999999996E-3</v>
+      </c>
+      <c r="H44">
+        <f>0.0721*11</f>
+        <v>0.79309999999999992</v>
+      </c>
+      <c r="I44" s="2">
+        <v>-0.82440000000000002</v>
+      </c>
+      <c r="J44">
+        <f>2014*-0.00163</f>
+        <v>-3.2828200000000001</v>
+      </c>
+      <c r="K44">
+        <f>SUM(B44:J44)</f>
+        <v>-2.7887900000000001</v>
+      </c>
+      <c r="L44">
+        <f>EXP(K44)</f>
+        <v>6.1495578565377643E-2</v>
+      </c>
+      <c r="M44">
+        <f>L44/(L44+1)</f>
+        <v>5.7932957807030679E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A47" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B47" t="s">
+        <v>4</v>
+      </c>
+      <c r="C47" t="s">
+        <v>60</v>
+      </c>
+      <c r="D47" t="s">
+        <v>6</v>
+      </c>
+      <c r="E47" t="s">
+        <v>62</v>
+      </c>
+      <c r="F47" t="s">
+        <v>7</v>
+      </c>
+      <c r="G47" t="s">
+        <v>8</v>
+      </c>
+      <c r="H47" t="s">
+        <v>33</v>
+      </c>
+      <c r="I47" t="s">
+        <v>29</v>
+      </c>
+      <c r="J47" t="s">
+        <v>61</v>
+      </c>
+      <c r="K47" t="s">
+        <v>11</v>
+      </c>
+      <c r="L47" t="s">
+        <v>52</v>
+      </c>
+      <c r="M47" t="s">
+        <v>12</v>
+      </c>
+      <c r="N47" t="s">
+        <v>13</v>
+      </c>
+      <c r="O47" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>59</v>
+      </c>
+      <c r="B48" s="5">
+        <v>-21.0091</v>
+      </c>
+      <c r="E48" s="5"/>
+      <c r="F48" s="5"/>
+      <c r="G48" s="5"/>
+      <c r="H48" s="5"/>
+      <c r="I48">
+        <f>18*0.0496</f>
+        <v>0.89279999999999993</v>
+      </c>
+      <c r="L48" s="5">
+        <f t="shared" ref="L48:L53" si="4">2015*0.00994</f>
+        <v>20.0291</v>
+      </c>
+      <c r="M48">
+        <f t="shared" ref="M48:M55" si="5">SUM(B48:L48)</f>
+        <v>-8.7199999999999278E-2</v>
+      </c>
+      <c r="N48">
+        <f t="shared" ref="N48:N55" si="6">EXP(M48)</f>
+        <v>0.91649377854634606</v>
+      </c>
+      <c r="O48">
+        <f t="shared" ref="O48:O55" si="7">N48/(N48+1)</f>
+        <v>0.47821380314706968</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>63</v>
+      </c>
+      <c r="B49" s="5">
+        <v>-21.0091</v>
+      </c>
+      <c r="E49" s="5"/>
+      <c r="F49" s="5"/>
+      <c r="G49" s="5"/>
+      <c r="H49" s="5"/>
+      <c r="J49">
+        <f>3*0.0496</f>
+        <v>0.14879999999999999</v>
+      </c>
+      <c r="L49" s="5">
+        <f t="shared" si="4"/>
+        <v>20.0291</v>
+      </c>
+      <c r="M49">
+        <f t="shared" si="5"/>
+        <v>-0.83119999999999905</v>
+      </c>
+      <c r="N49">
+        <f t="shared" si="6"/>
+        <v>0.43552634100789178</v>
+      </c>
+      <c r="O49">
+        <f t="shared" si="7"/>
+        <v>0.30339139628890827</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>64</v>
+      </c>
+      <c r="B50" s="5">
+        <v>-21.0091</v>
+      </c>
+      <c r="D50">
+        <v>-7.3099999999999998E-2</v>
+      </c>
+      <c r="E50" s="5"/>
+      <c r="F50" s="5"/>
+      <c r="G50" s="5"/>
+      <c r="H50" s="5"/>
+      <c r="I50">
+        <f t="shared" ref="I50:I55" si="8">18*0.0496</f>
+        <v>0.89279999999999993</v>
+      </c>
+      <c r="L50" s="5">
+        <f t="shared" si="4"/>
+        <v>20.0291</v>
+      </c>
+      <c r="M50">
+        <f t="shared" si="5"/>
+        <v>-0.16029999999999944</v>
+      </c>
+      <c r="N50">
+        <f t="shared" si="6"/>
+        <v>0.85188818417215806</v>
+      </c>
+      <c r="O50">
+        <f t="shared" si="7"/>
+        <v>0.46001059429674696</v>
       </c>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
+        <v>65</v>
+      </c>
+      <c r="B51" s="5">
+        <v>-21.0091</v>
+      </c>
+      <c r="C51">
+        <v>-0.50660000000000005</v>
+      </c>
+      <c r="E51" s="5"/>
+      <c r="F51" s="5"/>
+      <c r="G51" s="5"/>
+      <c r="H51" s="5"/>
+      <c r="I51">
+        <f t="shared" si="8"/>
+        <v>0.89279999999999993</v>
+      </c>
+      <c r="L51" s="5">
+        <f t="shared" si="4"/>
+        <v>20.0291</v>
+      </c>
+      <c r="M51">
+        <f t="shared" si="5"/>
+        <v>-0.59379999999999811</v>
+      </c>
+      <c r="N51">
+        <f t="shared" si="6"/>
+        <v>0.55222483823081736</v>
+      </c>
+      <c r="O51">
+        <f t="shared" si="7"/>
+        <v>0.3557634336403403</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>66</v>
+      </c>
+      <c r="B52" s="5">
+        <v>-21.0091</v>
+      </c>
+      <c r="E52" s="5">
+        <v>-0.81630000000000003</v>
+      </c>
+      <c r="F52" s="5"/>
+      <c r="G52" s="5"/>
+      <c r="H52" s="5"/>
+      <c r="I52">
+        <f t="shared" si="8"/>
+        <v>0.89279999999999993</v>
+      </c>
+      <c r="L52" s="5">
+        <f t="shared" si="4"/>
+        <v>20.0291</v>
+      </c>
+      <c r="M52">
+        <f t="shared" si="5"/>
+        <v>-0.90350000000000108</v>
+      </c>
+      <c r="N52">
+        <f t="shared" si="6"/>
+        <v>0.40514915326793383</v>
+      </c>
+      <c r="O52">
+        <f t="shared" si="7"/>
+        <v>0.28833177768045809</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>67</v>
+      </c>
+      <c r="B53" s="5">
+        <v>-21.0091</v>
+      </c>
+      <c r="E53" s="5"/>
+      <c r="F53" s="5">
+        <v>-0.48430000000000001</v>
+      </c>
+      <c r="G53" s="5"/>
+      <c r="H53" s="5"/>
+      <c r="I53">
+        <f t="shared" si="8"/>
+        <v>0.89279999999999993</v>
+      </c>
+      <c r="L53" s="5">
+        <f t="shared" si="4"/>
+        <v>20.0291</v>
+      </c>
+      <c r="M53">
+        <f t="shared" si="5"/>
+        <v>-0.57150000000000034</v>
+      </c>
+      <c r="N53">
+        <f t="shared" si="6"/>
+        <v>0.5646777864396173</v>
+      </c>
+      <c r="O53">
+        <f t="shared" si="7"/>
+        <v>0.36089077977167849</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>68</v>
+      </c>
+      <c r="B54" s="5">
+        <v>-21.0091</v>
+      </c>
+      <c r="E54" s="5"/>
+      <c r="F54" s="5"/>
+      <c r="G54" s="5"/>
+      <c r="H54" s="5"/>
+      <c r="I54">
+        <f t="shared" si="8"/>
+        <v>0.89279999999999993</v>
+      </c>
+      <c r="K54" s="5">
+        <f>2014*0.00994</f>
+        <v>20.019159999999999</v>
+      </c>
+      <c r="M54">
+        <f t="shared" si="5"/>
+        <v>-9.713999999999956E-2</v>
+      </c>
+      <c r="N54">
+        <f t="shared" si="6"/>
+        <v>0.90742895718604821</v>
+      </c>
+      <c r="O54">
+        <f t="shared" si="7"/>
+        <v>0.47573407846588478</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>69</v>
+      </c>
+      <c r="B55" s="5">
+        <v>-21.0091</v>
+      </c>
+      <c r="E55" s="5"/>
+      <c r="F55" s="5"/>
+      <c r="G55" s="5"/>
+      <c r="H55" s="5">
+        <v>2.5499999999999998E-2</v>
+      </c>
+      <c r="I55">
+        <f t="shared" si="8"/>
+        <v>0.89279999999999993</v>
+      </c>
+      <c r="L55" s="5">
+        <f>2015*0.00994</f>
+        <v>20.0291</v>
+      </c>
+      <c r="M55">
+        <f t="shared" si="5"/>
+        <v>-6.1699999999998312E-2</v>
+      </c>
+      <c r="N55">
+        <f t="shared" si="6"/>
+        <v>0.94016489395608749</v>
+      </c>
+      <c r="O55">
+        <f t="shared" si="7"/>
+        <v>0.48457989157769316</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A57" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B57" t="s">
+        <v>4</v>
+      </c>
+      <c r="C57" t="s">
+        <v>71</v>
+      </c>
+      <c r="D57" t="s">
+        <v>6</v>
+      </c>
+      <c r="E57" t="s">
+        <v>62</v>
+      </c>
+      <c r="F57" t="s">
+        <v>7</v>
+      </c>
+      <c r="G57" t="s">
+        <v>8</v>
+      </c>
+      <c r="H57" t="s">
+        <v>33</v>
+      </c>
+      <c r="I57" t="s">
+        <v>29</v>
+      </c>
+      <c r="J57" t="s">
         <v>34</v>
       </c>
+      <c r="K57" t="s">
+        <v>11</v>
+      </c>
+      <c r="L57" t="s">
+        <v>52</v>
+      </c>
+      <c r="M57" t="s">
+        <v>12</v>
+      </c>
+      <c r="N57" t="s">
+        <v>13</v>
+      </c>
+      <c r="O57" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>70</v>
+      </c>
+      <c r="B58" s="5">
+        <v>29.564</v>
+      </c>
+      <c r="I58">
+        <f>0.0424*18</f>
+        <v>0.76319999999999999</v>
+      </c>
+      <c r="L58">
+        <f>-0.0154*2015</f>
+        <v>-31.031000000000002</v>
+      </c>
+      <c r="M58">
+        <f t="shared" ref="M58:M65" si="9">SUM(B58:L58)</f>
+        <v>-0.70380000000000109</v>
+      </c>
+      <c r="N58">
+        <f t="shared" ref="N58:N65" si="10">EXP(M58)</f>
+        <v>0.49470186044576797</v>
+      </c>
+      <c r="O58">
+        <f t="shared" ref="O58:O65" si="11">N58/(N58+1)</f>
+        <v>0.33097025804077879</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>78</v>
+      </c>
+      <c r="B59" s="5">
+        <v>29.564</v>
+      </c>
+      <c r="E59" s="5"/>
+      <c r="F59" s="5"/>
+      <c r="G59" s="5"/>
+      <c r="H59" s="5"/>
+      <c r="J59">
+        <f>0.0424*13</f>
+        <v>0.55120000000000002</v>
+      </c>
+      <c r="L59">
+        <f t="shared" ref="L59:L65" si="12">-0.0154*2015</f>
+        <v>-31.031000000000002</v>
+      </c>
+      <c r="M59">
+        <f t="shared" si="9"/>
+        <v>-0.91580000000000084</v>
+      </c>
+      <c r="N59">
+        <f t="shared" si="10"/>
+        <v>0.40019634092109557</v>
+      </c>
+      <c r="O59">
+        <f t="shared" si="11"/>
+        <v>0.28581444560684477</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>72</v>
+      </c>
+      <c r="B60" s="5">
+        <v>29.564</v>
+      </c>
+      <c r="D60">
+        <v>-2.76E-2</v>
+      </c>
+      <c r="E60" s="5"/>
+      <c r="F60" s="5"/>
+      <c r="G60" s="5"/>
+      <c r="H60" s="5"/>
+      <c r="I60">
+        <f t="shared" ref="I60:I65" si="13">0.0424*18</f>
+        <v>0.76319999999999999</v>
+      </c>
+      <c r="L60">
+        <f t="shared" si="12"/>
+        <v>-31.031000000000002</v>
+      </c>
+      <c r="M60">
+        <f t="shared" si="9"/>
+        <v>-0.73140000000000072</v>
+      </c>
+      <c r="N60">
+        <f t="shared" si="10"/>
+        <v>0.48123478955457016</v>
+      </c>
+      <c r="O60">
+        <f t="shared" si="11"/>
+        <v>0.32488758227133241</v>
+      </c>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A61" s="4" t="s">
-        <v>42</v>
+      <c r="A61" t="s">
+        <v>77</v>
+      </c>
+      <c r="B61" s="5">
+        <v>29.564</v>
+      </c>
+      <c r="C61">
+        <v>-0.70169999999999999</v>
+      </c>
+      <c r="E61" s="5"/>
+      <c r="F61" s="5"/>
+      <c r="G61" s="5"/>
+      <c r="H61" s="5"/>
+      <c r="I61">
+        <f t="shared" si="13"/>
+        <v>0.76319999999999999</v>
+      </c>
+      <c r="L61">
+        <f t="shared" si="12"/>
+        <v>-31.031000000000002</v>
+      </c>
+      <c r="M61">
+        <f t="shared" si="9"/>
+        <v>-1.4055</v>
+      </c>
+      <c r="N61">
+        <f t="shared" si="10"/>
+        <v>0.24524440359047078</v>
+      </c>
+      <c r="O61">
+        <f t="shared" si="11"/>
+        <v>0.19694479483974892</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>73</v>
+      </c>
+      <c r="B62" s="5">
+        <v>29.564</v>
+      </c>
+      <c r="E62" s="5">
+        <v>-0.2082</v>
+      </c>
+      <c r="F62" s="5"/>
+      <c r="G62" s="5"/>
+      <c r="H62" s="5"/>
+      <c r="I62">
+        <f t="shared" si="13"/>
+        <v>0.76319999999999999</v>
+      </c>
+      <c r="L62">
+        <f t="shared" si="12"/>
+        <v>-31.031000000000002</v>
+      </c>
+      <c r="M62">
+        <f t="shared" si="9"/>
+        <v>-0.91200000000000259</v>
+      </c>
+      <c r="N62">
+        <f t="shared" si="10"/>
+        <v>0.40171998009758503</v>
+      </c>
+      <c r="O62">
+        <f t="shared" si="11"/>
+        <v>0.28659074979413368</v>
       </c>
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B63" t="s">
-        <v>4</v>
-      </c>
-      <c r="C63" t="s">
-        <v>6</v>
-      </c>
-      <c r="D63" t="s">
-        <v>7</v>
-      </c>
-      <c r="E63" t="s">
-        <v>8</v>
-      </c>
-      <c r="F63" t="s">
-        <v>35</v>
-      </c>
-      <c r="G63" t="s">
-        <v>29</v>
-      </c>
-      <c r="H63" t="s">
-        <v>36</v>
-      </c>
-      <c r="I63" t="s">
-        <v>26</v>
-      </c>
-      <c r="J63" t="s">
-        <v>55</v>
-      </c>
-      <c r="K63" t="s">
-        <v>11</v>
-      </c>
-      <c r="L63" t="s">
-        <v>54</v>
-      </c>
-      <c r="M63" t="s">
-        <v>12</v>
-      </c>
-      <c r="N63" t="s">
-        <v>13</v>
-      </c>
-      <c r="O63" t="s">
-        <v>14</v>
+      <c r="A63" t="s">
+        <v>74</v>
+      </c>
+      <c r="B63" s="5">
+        <v>29.564</v>
+      </c>
+      <c r="E63" s="5"/>
+      <c r="F63" s="5">
+        <v>-0.43090000000000001</v>
+      </c>
+      <c r="G63" s="5"/>
+      <c r="H63" s="5"/>
+      <c r="I63">
+        <f t="shared" si="13"/>
+        <v>0.76319999999999999</v>
+      </c>
+      <c r="L63">
+        <f t="shared" si="12"/>
+        <v>-31.031000000000002</v>
+      </c>
+      <c r="M63">
+        <f t="shared" si="9"/>
+        <v>-1.1347000000000023</v>
+      </c>
+      <c r="N63">
+        <f t="shared" si="10"/>
+        <v>0.32151856243623289</v>
+      </c>
+      <c r="O63">
+        <f t="shared" si="11"/>
+        <v>0.24329477585506643</v>
       </c>
     </row>
     <row r="64" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>57</v>
-      </c>
-      <c r="B64" s="3">
-        <v>2.7008999999999999</v>
-      </c>
-      <c r="F64" s="3"/>
-      <c r="G64">
-        <f>0.0123*18</f>
-        <v>0.22140000000000001</v>
-      </c>
-      <c r="I64" s="3"/>
-      <c r="L64" s="3">
-        <f>2015*-0.00177</f>
-        <v>-3.5665500000000003</v>
+        <v>75</v>
+      </c>
+      <c r="B64" s="5">
+        <v>29.564</v>
+      </c>
+      <c r="E64" s="5"/>
+      <c r="F64" s="5"/>
+      <c r="G64" s="5"/>
+      <c r="H64" s="5"/>
+      <c r="I64">
+        <f t="shared" si="13"/>
+        <v>0.76319999999999999</v>
+      </c>
+      <c r="K64">
+        <f>-0.0154*2014</f>
+        <v>-31.015600000000003</v>
       </c>
       <c r="M64">
-        <f>SUM(B64:L64)</f>
-        <v>-0.64425000000000043</v>
+        <f t="shared" si="9"/>
+        <v>-0.68840000000000146</v>
       </c>
       <c r="N64">
-        <f>EXP(M64)</f>
-        <v>0.52505618661140985</v>
+        <f t="shared" si="10"/>
+        <v>0.50237923313647515</v>
       </c>
       <c r="O64">
-        <f>N64/(N64+1)</f>
-        <v>0.3442864539817746</v>
-      </c>
-    </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
+        <f t="shared" si="11"/>
+        <v>0.33438909567970537</v>
+      </c>
+    </row>
+    <row r="65" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>56</v>
-      </c>
-      <c r="B65" s="3">
-        <v>2.7008999999999999</v>
-      </c>
-      <c r="C65" s="3"/>
-      <c r="F65" s="3"/>
-      <c r="H65">
-        <f>0.0123*13</f>
-        <v>0.15990000000000001</v>
-      </c>
-      <c r="I65" s="3"/>
-      <c r="K65" s="3"/>
-      <c r="L65" s="3">
-        <f>2015*-0.00177</f>
-        <v>-3.5665500000000003</v>
+        <v>76</v>
+      </c>
+      <c r="B65" s="5">
+        <v>29.564</v>
+      </c>
+      <c r="E65" s="5"/>
+      <c r="F65" s="5"/>
+      <c r="G65" s="5"/>
+      <c r="H65" s="5">
+        <v>-1.4E-2</v>
+      </c>
+      <c r="I65">
+        <f t="shared" si="13"/>
+        <v>0.76319999999999999</v>
+      </c>
+      <c r="L65">
+        <f t="shared" si="12"/>
+        <v>-31.031000000000002</v>
       </c>
       <c r="M65">
-        <f>SUM(B65:L65)</f>
-        <v>-0.70575000000000054</v>
+        <f t="shared" si="9"/>
+        <v>-0.71780000000000044</v>
       </c>
       <c r="N65">
-        <f>EXP(M65)</f>
-        <v>0.49373813175875031</v>
+        <f t="shared" si="10"/>
+        <v>0.48782428972784109</v>
       </c>
       <c r="O65">
-        <f>N65/(N65+1)</f>
-        <v>0.33053861400553214</v>
-      </c>
-    </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>58</v>
-      </c>
-      <c r="B66" s="3">
-        <v>2.7008999999999999</v>
-      </c>
-      <c r="C66" s="3">
-        <v>-6.4000000000000001E-2</v>
-      </c>
-      <c r="D66" s="3"/>
-      <c r="G66">
-        <f>0.0123*18</f>
-        <v>0.22140000000000001</v>
-      </c>
-      <c r="L66" s="3">
-        <f>2015*-0.00177</f>
-        <v>-3.5665500000000003</v>
-      </c>
-      <c r="M66">
-        <f>SUM(B66:L66)</f>
-        <v>-0.70825000000000049</v>
-      </c>
-      <c r="N66">
-        <f>EXP(M66)</f>
-        <v>0.49250532807604203</v>
-      </c>
-      <c r="O66">
-        <f>N66/(N66+1)</f>
-        <v>0.32998564146562914</v>
-      </c>
-    </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>59</v>
-      </c>
-      <c r="B67" s="3">
-        <v>2.7008999999999999</v>
-      </c>
-      <c r="D67" s="3">
-        <v>-0.13669999999999999</v>
-      </c>
-      <c r="G67">
-        <f>0.0123*18</f>
-        <v>0.22140000000000001</v>
-      </c>
-      <c r="L67" s="3">
-        <f>2015*-0.00177</f>
-        <v>-3.5665500000000003</v>
-      </c>
-      <c r="M67">
-        <f>SUM(B67:L67)</f>
-        <v>-0.78095000000000026</v>
-      </c>
-      <c r="N67">
-        <f>EXP(M67)</f>
-        <v>0.45797073238470731</v>
-      </c>
-      <c r="O67">
-        <f>N67/(N67+1)</f>
-        <v>0.31411517543677614</v>
-      </c>
-    </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A70" s="4" t="s">
+        <f t="shared" si="11"/>
+        <v>0.32787762177015939</v>
+      </c>
+    </row>
+    <row r="67" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A67" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B67" t="s">
+        <v>4</v>
+      </c>
+      <c r="C67" t="s">
+        <v>80</v>
+      </c>
+      <c r="D67" t="s">
+        <v>81</v>
+      </c>
+      <c r="E67" t="s">
+        <v>82</v>
+      </c>
+      <c r="F67" t="s">
+        <v>83</v>
+      </c>
+      <c r="G67" t="s">
+        <v>6</v>
+      </c>
+      <c r="H67" t="s">
+        <v>62</v>
+      </c>
+      <c r="I67" t="s">
+        <v>7</v>
+      </c>
+      <c r="J67" t="s">
+        <v>8</v>
+      </c>
+      <c r="K67" t="s">
+        <v>33</v>
+      </c>
+      <c r="L67" t="s">
+        <v>29</v>
+      </c>
+      <c r="M67" t="s">
+        <v>34</v>
+      </c>
+      <c r="N67" t="s">
+        <v>11</v>
+      </c>
+      <c r="O67" t="s">
+        <v>52</v>
+      </c>
+      <c r="P67" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q67" t="s">
+        <v>13</v>
+      </c>
+      <c r="R67" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="68" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>79</v>
+      </c>
+      <c r="B68" s="5">
+        <v>-36.502800000000001</v>
+      </c>
+      <c r="L68">
+        <f>0.0215*18</f>
+        <v>0.38699999999999996</v>
+      </c>
+      <c r="O68">
+        <f>0.0179*2015</f>
+        <v>36.0685</v>
+      </c>
+      <c r="P68">
+        <f t="shared" ref="P68:P78" si="14">SUM(B68:O68)</f>
+        <v>-4.7299999999999898E-2</v>
+      </c>
+      <c r="Q68">
+        <f t="shared" ref="Q68:Q74" si="15">EXP(P68)</f>
+        <v>0.95380121430073395</v>
+      </c>
+      <c r="R68">
+        <f t="shared" ref="R68:R74" si="16">Q68/(Q68+1)</f>
+        <v>0.48817720416971883</v>
+      </c>
+    </row>
+    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>84</v>
+      </c>
+      <c r="B69" s="5">
+        <v>-36.502800000000001</v>
+      </c>
+      <c r="H69" s="5"/>
+      <c r="I69" s="5"/>
+      <c r="J69" s="5"/>
+      <c r="K69" s="5"/>
+      <c r="M69">
+        <f>0.0215*13</f>
+        <v>0.27949999999999997</v>
+      </c>
+      <c r="O69">
+        <f t="shared" ref="O69:O78" si="17">0.0179*2015</f>
+        <v>36.0685</v>
+      </c>
+      <c r="P69">
+        <f t="shared" si="14"/>
+        <v>-0.1548000000000016</v>
+      </c>
+      <c r="Q69">
+        <f t="shared" si="15"/>
+        <v>0.85658647764855433</v>
+      </c>
+      <c r="R69">
+        <f t="shared" si="16"/>
+        <v>0.46137709606366278</v>
+      </c>
+    </row>
+    <row r="70" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>85</v>
+      </c>
+      <c r="B70" s="5">
+        <v>-36.502800000000001</v>
+      </c>
+      <c r="G70" s="6">
+        <v>-1.1900000000000001E-2</v>
+      </c>
+      <c r="H70" s="5"/>
+      <c r="I70" s="5"/>
+      <c r="J70" s="5"/>
+      <c r="K70" s="5"/>
+      <c r="L70">
+        <f t="shared" ref="L70:L78" si="18">0.0215*18</f>
+        <v>0.38699999999999996</v>
+      </c>
+      <c r="O70">
+        <f t="shared" si="17"/>
+        <v>36.0685</v>
+      </c>
+      <c r="P70">
+        <f t="shared" si="14"/>
+        <v>-5.9199999999997033E-2</v>
+      </c>
+      <c r="Q70">
+        <f t="shared" si="15"/>
+        <v>0.94251824665614958</v>
+      </c>
+      <c r="R70">
+        <f t="shared" si="16"/>
+        <v>0.48520432087502924</v>
+      </c>
+    </row>
+    <row r="71" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>86</v>
+      </c>
+      <c r="B71" s="5">
+        <v>-36.502800000000001</v>
+      </c>
+      <c r="H71" s="6">
+        <v>-1.0116000000000001</v>
+      </c>
+      <c r="I71" s="5"/>
+      <c r="J71" s="5"/>
+      <c r="K71" s="5"/>
+      <c r="L71">
+        <f t="shared" si="18"/>
+        <v>0.38699999999999996</v>
+      </c>
+      <c r="O71">
+        <f t="shared" si="17"/>
+        <v>36.0685</v>
+      </c>
+      <c r="P71">
+        <f t="shared" si="14"/>
+        <v>-1.0589000000000013</v>
+      </c>
+      <c r="Q71">
+        <f t="shared" si="15"/>
+        <v>0.34683712140406192</v>
+      </c>
+      <c r="R71">
+        <f t="shared" si="16"/>
+        <v>0.25751972223819336</v>
+      </c>
+    </row>
+    <row r="72" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>87</v>
+      </c>
+      <c r="B72" s="5">
+        <v>-36.502800000000001</v>
+      </c>
+      <c r="H72" s="5"/>
+      <c r="I72" s="6">
+        <v>-0.57979999999999998</v>
+      </c>
+      <c r="J72" s="5"/>
+      <c r="K72" s="5"/>
+      <c r="L72">
+        <f t="shared" si="18"/>
+        <v>0.38699999999999996</v>
+      </c>
+      <c r="O72">
+        <f t="shared" si="17"/>
+        <v>36.0685</v>
+      </c>
+      <c r="P72">
+        <f t="shared" si="14"/>
+        <v>-0.62709999999999866</v>
+      </c>
+      <c r="Q72">
+        <f t="shared" si="15"/>
+        <v>0.53413855894480855</v>
+      </c>
+      <c r="R72">
+        <f t="shared" si="16"/>
+        <v>0.34816839445857667</v>
+      </c>
+    </row>
+    <row r="73" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>88</v>
+      </c>
+      <c r="B73" s="5">
+        <v>-36.502800000000001</v>
+      </c>
+      <c r="H73" s="5"/>
+      <c r="I73" s="5"/>
+      <c r="J73" s="5"/>
+      <c r="K73" s="5"/>
+      <c r="L73">
+        <f t="shared" si="18"/>
+        <v>0.38699999999999996</v>
+      </c>
+      <c r="N73">
+        <f>0.0179*2014</f>
+        <v>36.050599999999996</v>
+      </c>
+      <c r="P73">
+        <f t="shared" si="14"/>
+        <v>-6.5200000000004366E-2</v>
+      </c>
+      <c r="Q73">
+        <f t="shared" si="15"/>
+        <v>0.93688006862482376</v>
+      </c>
+      <c r="R73">
+        <f t="shared" si="16"/>
+        <v>0.48370577187569719</v>
+      </c>
+    </row>
+    <row r="74" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>89</v>
+      </c>
+      <c r="B74" s="5">
+        <v>-36.502800000000001</v>
+      </c>
+      <c r="H74" s="5"/>
+      <c r="I74" s="5"/>
+      <c r="J74" s="5"/>
+      <c r="K74" s="6">
+        <v>-9.8899999999999995E-3</v>
+      </c>
+      <c r="L74">
+        <f t="shared" si="18"/>
+        <v>0.38699999999999996</v>
+      </c>
+      <c r="O74">
+        <f t="shared" si="17"/>
+        <v>36.0685</v>
+      </c>
+      <c r="P74">
+        <f t="shared" si="14"/>
+        <v>-5.718999999999852E-2</v>
+      </c>
+      <c r="Q74">
+        <f t="shared" si="15"/>
+        <v>0.94441461354218825</v>
+      </c>
+      <c r="R74">
+        <f t="shared" si="16"/>
+        <v>0.48570639562398926</v>
+      </c>
+    </row>
+    <row r="75" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>90</v>
+      </c>
+      <c r="B75" s="5">
+        <v>-36.502800000000001</v>
+      </c>
+      <c r="C75" s="6">
+        <v>-8.8800000000000004E-2</v>
+      </c>
+      <c r="H75" s="5"/>
+      <c r="I75" s="5"/>
+      <c r="J75" s="5"/>
+      <c r="K75" s="5"/>
+      <c r="L75">
+        <f t="shared" si="18"/>
+        <v>0.38699999999999996</v>
+      </c>
+      <c r="O75">
+        <f t="shared" si="17"/>
+        <v>36.0685</v>
+      </c>
+      <c r="P75">
+        <f t="shared" si="14"/>
+        <v>-0.136099999999999</v>
+      </c>
+      <c r="Q75">
+        <f>EXP(P75)</f>
+        <v>0.87275535258953907</v>
+      </c>
+      <c r="R75">
+        <f>Q75/(Q75+1)</f>
+        <v>0.46602742391457747</v>
+      </c>
+    </row>
+    <row r="76" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>91</v>
+      </c>
+      <c r="B76" s="5">
+        <v>-36.502800000000001</v>
+      </c>
+      <c r="D76" s="6">
+        <v>0.59689999999999999</v>
+      </c>
+      <c r="H76" s="5"/>
+      <c r="I76" s="5"/>
+      <c r="J76" s="5"/>
+      <c r="K76" s="5"/>
+      <c r="L76">
+        <f t="shared" si="18"/>
+        <v>0.38699999999999996</v>
+      </c>
+      <c r="O76">
+        <f t="shared" si="17"/>
+        <v>36.0685</v>
+      </c>
+      <c r="P76">
+        <f t="shared" si="14"/>
+        <v>0.54959999999999809</v>
+      </c>
+      <c r="Q76">
+        <f>EXP(P76)</f>
+        <v>1.7325598553020003</v>
+      </c>
+      <c r="R76">
+        <f>Q76/(Q76+1)</f>
+        <v>0.63404278297520378</v>
+      </c>
+    </row>
+    <row r="77" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>92</v>
+      </c>
+      <c r="B77" s="5">
+        <v>-36.502800000000001</v>
+      </c>
+      <c r="E77" s="6">
+        <v>-0.1613</v>
+      </c>
+      <c r="H77" s="5"/>
+      <c r="I77" s="5"/>
+      <c r="J77" s="5"/>
+      <c r="K77" s="5"/>
+      <c r="L77">
+        <f t="shared" si="18"/>
+        <v>0.38699999999999996</v>
+      </c>
+      <c r="O77">
+        <f t="shared" si="17"/>
+        <v>36.0685</v>
+      </c>
+      <c r="P77">
+        <f t="shared" si="14"/>
+        <v>-0.20859999999999701</v>
+      </c>
+      <c r="Q77">
+        <f>EXP(P77)</f>
+        <v>0.81171985865794583</v>
+      </c>
+      <c r="R77">
+        <f>Q77/(Q77+1)</f>
+        <v>0.44803828515697647</v>
+      </c>
+    </row>
+    <row r="78" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>93</v>
+      </c>
+      <c r="B78" s="5">
+        <v>-36.502800000000001</v>
+      </c>
+      <c r="F78" s="6">
+        <v>-0.3196</v>
+      </c>
+      <c r="H78" s="5"/>
+      <c r="I78" s="5"/>
+      <c r="J78" s="5"/>
+      <c r="K78" s="5"/>
+      <c r="L78">
+        <f t="shared" si="18"/>
+        <v>0.38699999999999996</v>
+      </c>
+      <c r="O78">
+        <f t="shared" si="17"/>
+        <v>36.0685</v>
+      </c>
+      <c r="P78">
+        <f t="shared" si="14"/>
+        <v>-0.36690000000000111</v>
+      </c>
+      <c r="Q78">
+        <f>EXP(P78)</f>
+        <v>0.69287892947305907</v>
+      </c>
+      <c r="R78">
+        <f>Q78/(Q78+1)</f>
+        <v>0.40929030269679761</v>
+      </c>
+    </row>
+    <row r="79" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B79" s="5"/>
+      <c r="H79" s="5"/>
+      <c r="I79" s="5"/>
+      <c r="J79" s="5"/>
+      <c r="K79" s="5"/>
+    </row>
+    <row r="84" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A84" s="4" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B73" t="s">
+      <c r="B84" t="s">
         <v>4</v>
       </c>
-      <c r="C73" t="s">
-        <v>32</v>
-      </c>
-      <c r="D73" t="s">
+      <c r="C84" t="s">
+        <v>102</v>
+      </c>
+      <c r="D84" t="s">
         <v>6</v>
       </c>
-      <c r="E73" t="s">
+      <c r="E84" t="s">
+        <v>62</v>
+      </c>
+      <c r="F84" t="s">
         <v>7</v>
       </c>
-      <c r="F73" t="s">
+      <c r="G84" t="s">
         <v>8</v>
       </c>
-      <c r="G73" t="s">
-        <v>35</v>
-      </c>
-      <c r="H73" t="s">
-        <v>10</v>
-      </c>
-      <c r="I73" t="s">
-        <v>26</v>
-      </c>
-      <c r="J73" t="s">
+      <c r="H84" t="s">
+        <v>33</v>
+      </c>
+      <c r="I84" t="s">
+        <v>29</v>
+      </c>
+      <c r="J84" t="s">
+        <v>34</v>
+      </c>
+      <c r="K84" t="s">
         <v>11</v>
       </c>
-      <c r="K73" t="s">
+      <c r="L84" t="s">
+        <v>52</v>
+      </c>
+      <c r="M84" t="s">
         <v>12</v>
       </c>
-      <c r="L73" t="s">
+      <c r="N84" t="s">
         <v>13</v>
       </c>
-      <c r="M73" t="s">
+      <c r="O84" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>31</v>
-      </c>
-      <c r="B74" s="2">
-        <v>1.3971</v>
-      </c>
-      <c r="C74" s="2">
-        <v>-8.6199999999999999E-2</v>
-      </c>
-      <c r="D74" s="2">
-        <v>-9.1499999999999998E-2</v>
-      </c>
-      <c r="E74" s="2">
-        <v>-0.68579999999999997</v>
-      </c>
-      <c r="G74" s="2">
-        <v>-8.2699999999999996E-3</v>
-      </c>
-      <c r="H74">
-        <f>0.0721*11</f>
-        <v>0.79309999999999992</v>
-      </c>
-      <c r="I74" s="2">
-        <v>-0.82440000000000002</v>
-      </c>
-      <c r="J74">
-        <f>2014*-0.00163</f>
-        <v>-3.2828200000000001</v>
-      </c>
-      <c r="K74">
-        <f>SUM(B74:J74)</f>
-        <v>-2.7887900000000001</v>
-      </c>
-      <c r="L74">
-        <f>EXP(K74)</f>
-        <v>6.1495578565377643E-2</v>
-      </c>
-      <c r="M74">
-        <f>L74/(L74+1)</f>
-        <v>5.7932957807030679E-2</v>
-      </c>
-    </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A77" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B77" t="s">
-        <v>4</v>
-      </c>
-      <c r="C77" t="s">
-        <v>62</v>
-      </c>
-      <c r="D77" t="s">
-        <v>6</v>
-      </c>
-      <c r="E77" t="s">
-        <v>64</v>
-      </c>
-      <c r="F77" t="s">
-        <v>7</v>
-      </c>
-      <c r="G77" t="s">
-        <v>8</v>
-      </c>
-      <c r="H77" t="s">
-        <v>35</v>
-      </c>
-      <c r="I77" t="s">
-        <v>29</v>
-      </c>
-      <c r="J77" t="s">
-        <v>63</v>
-      </c>
-      <c r="K77" t="s">
-        <v>11</v>
-      </c>
-      <c r="L77" t="s">
-        <v>54</v>
-      </c>
-      <c r="M77" t="s">
-        <v>12</v>
-      </c>
-      <c r="N77" t="s">
-        <v>13</v>
-      </c>
-      <c r="O77" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>61</v>
-      </c>
-      <c r="B78" s="5">
-        <v>-21.0091</v>
-      </c>
-      <c r="E78" s="5"/>
-      <c r="F78" s="5"/>
-      <c r="G78" s="5"/>
-      <c r="H78" s="5"/>
-      <c r="I78">
-        <f>18*0.0496</f>
-        <v>0.89279999999999993</v>
-      </c>
-      <c r="L78" s="5">
-        <f t="shared" ref="L78:L83" si="4">2015*0.00994</f>
-        <v>20.0291</v>
-      </c>
-      <c r="M78">
-        <f t="shared" ref="M78:M85" si="5">SUM(B78:L78)</f>
-        <v>-8.7199999999999278E-2</v>
-      </c>
-      <c r="N78">
-        <f t="shared" ref="N78:N85" si="6">EXP(M78)</f>
-        <v>0.91649377854634606</v>
-      </c>
-      <c r="O78">
-        <f t="shared" ref="O78:O85" si="7">N78/(N78+1)</f>
-        <v>0.47821380314706968</v>
-      </c>
-    </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>65</v>
-      </c>
-      <c r="B79" s="5">
-        <v>-21.0091</v>
-      </c>
-      <c r="E79" s="5"/>
-      <c r="F79" s="5"/>
-      <c r="G79" s="5"/>
-      <c r="H79" s="5"/>
-      <c r="J79">
-        <f>3*0.0496</f>
-        <v>0.14879999999999999</v>
-      </c>
-      <c r="L79" s="5">
-        <f t="shared" si="4"/>
-        <v>20.0291</v>
-      </c>
-      <c r="M79">
-        <f t="shared" si="5"/>
-        <v>-0.83119999999999905</v>
-      </c>
-      <c r="N79">
-        <f t="shared" si="6"/>
-        <v>0.43552634100789178</v>
-      </c>
-      <c r="O79">
-        <f t="shared" si="7"/>
-        <v>0.30339139628890827</v>
-      </c>
-    </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
-        <v>66</v>
-      </c>
-      <c r="B80" s="5">
-        <v>-21.0091</v>
-      </c>
-      <c r="D80">
-        <v>-7.3099999999999998E-2</v>
-      </c>
-      <c r="E80" s="5"/>
-      <c r="F80" s="5"/>
-      <c r="G80" s="5"/>
-      <c r="H80" s="5"/>
-      <c r="I80">
-        <f t="shared" ref="I80:I85" si="8">18*0.0496</f>
-        <v>0.89279999999999993</v>
-      </c>
-      <c r="L80" s="5">
-        <f t="shared" si="4"/>
-        <v>20.0291</v>
-      </c>
-      <c r="M80">
-        <f t="shared" si="5"/>
-        <v>-0.16029999999999944</v>
-      </c>
-      <c r="N80">
-        <f t="shared" si="6"/>
-        <v>0.85188818417215806</v>
-      </c>
-      <c r="O80">
-        <f t="shared" si="7"/>
-        <v>0.46001059429674696</v>
-      </c>
-    </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
-        <v>67</v>
-      </c>
-      <c r="B81" s="5">
-        <v>-21.0091</v>
-      </c>
-      <c r="C81">
-        <v>-0.50660000000000005</v>
-      </c>
-      <c r="E81" s="5"/>
-      <c r="F81" s="5"/>
-      <c r="G81" s="5"/>
-      <c r="H81" s="5"/>
-      <c r="I81">
-        <f t="shared" si="8"/>
-        <v>0.89279999999999993</v>
-      </c>
-      <c r="L81" s="5">
-        <f t="shared" si="4"/>
-        <v>20.0291</v>
-      </c>
-      <c r="M81">
-        <f t="shared" si="5"/>
-        <v>-0.59379999999999811</v>
-      </c>
-      <c r="N81">
-        <f t="shared" si="6"/>
-        <v>0.55222483823081736</v>
-      </c>
-      <c r="O81">
-        <f t="shared" si="7"/>
-        <v>0.3557634336403403</v>
-      </c>
-    </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
-        <v>68</v>
-      </c>
-      <c r="B82" s="5">
-        <v>-21.0091</v>
-      </c>
-      <c r="E82" s="5">
-        <v>-0.81630000000000003</v>
-      </c>
-      <c r="F82" s="5"/>
-      <c r="G82" s="5"/>
-      <c r="H82" s="5"/>
-      <c r="I82">
-        <f t="shared" si="8"/>
-        <v>0.89279999999999993</v>
-      </c>
-      <c r="L82" s="5">
-        <f t="shared" si="4"/>
-        <v>20.0291</v>
-      </c>
-      <c r="M82">
-        <f t="shared" si="5"/>
-        <v>-0.90350000000000108</v>
-      </c>
-      <c r="N82">
-        <f t="shared" si="6"/>
-        <v>0.40514915326793383</v>
-      </c>
-      <c r="O82">
-        <f t="shared" si="7"/>
-        <v>0.28833177768045809</v>
-      </c>
-    </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
-        <v>69</v>
-      </c>
-      <c r="B83" s="5">
-        <v>-21.0091</v>
-      </c>
-      <c r="E83" s="5"/>
-      <c r="F83" s="5">
-        <v>-0.48430000000000001</v>
-      </c>
-      <c r="G83" s="5"/>
-      <c r="H83" s="5"/>
-      <c r="I83">
-        <f t="shared" si="8"/>
-        <v>0.89279999999999993</v>
-      </c>
-      <c r="L83" s="5">
-        <f t="shared" si="4"/>
-        <v>20.0291</v>
-      </c>
-      <c r="M83">
-        <f t="shared" si="5"/>
-        <v>-0.57150000000000034</v>
-      </c>
-      <c r="N83">
-        <f t="shared" si="6"/>
-        <v>0.5646777864396173</v>
-      </c>
-      <c r="O83">
-        <f t="shared" si="7"/>
-        <v>0.36089077977167849</v>
-      </c>
-    </row>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
-        <v>70</v>
-      </c>
-      <c r="B84" s="5">
-        <v>-21.0091</v>
-      </c>
-      <c r="E84" s="5"/>
-      <c r="F84" s="5"/>
-      <c r="G84" s="5"/>
-      <c r="H84" s="5"/>
-      <c r="I84">
-        <f t="shared" si="8"/>
-        <v>0.89279999999999993</v>
-      </c>
-      <c r="K84" s="5">
-        <f>2014*0.00994</f>
-        <v>20.019159999999999</v>
-      </c>
-      <c r="M84">
-        <f t="shared" si="5"/>
-        <v>-9.713999999999956E-2</v>
-      </c>
-      <c r="N84">
-        <f t="shared" si="6"/>
-        <v>0.90742895718604821</v>
-      </c>
-      <c r="O84">
-        <f t="shared" si="7"/>
-        <v>0.47573407846588478</v>
       </c>
     </row>
     <row r="85" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>71</v>
-      </c>
-      <c r="B85" s="5">
-        <v>-21.0091</v>
-      </c>
-      <c r="E85" s="5"/>
-      <c r="F85" s="5"/>
-      <c r="G85" s="5"/>
-      <c r="H85" s="5">
-        <v>2.5499999999999998E-2</v>
+        <v>95</v>
+      </c>
+      <c r="B85" s="7">
+        <v>1.3971</v>
       </c>
       <c r="I85">
-        <f t="shared" si="8"/>
-        <v>0.89279999999999993</v>
-      </c>
-      <c r="L85" s="5">
-        <f>2015*0.00994</f>
-        <v>20.0291</v>
+        <f>0.0721*18</f>
+        <v>1.2978000000000001</v>
+      </c>
+      <c r="L85">
+        <f t="shared" ref="L85:L89" si="19">-0.00163*2015</f>
+        <v>-3.2844500000000001</v>
       </c>
       <c r="M85">
-        <f t="shared" si="5"/>
-        <v>-6.1699999999998312E-2</v>
+        <f t="shared" ref="M85:M92" si="20">SUM(B85:L85)</f>
+        <v>-0.58955000000000002</v>
       </c>
       <c r="N85">
-        <f t="shared" si="6"/>
-        <v>0.94016489395608749</v>
+        <f t="shared" ref="N85:N91" si="21">EXP(M85)</f>
+        <v>0.55457678814669498</v>
       </c>
       <c r="O85">
-        <f t="shared" si="7"/>
-        <v>0.48457989157769316</v>
+        <f t="shared" ref="O85:O91" si="22">N85/(N85+1)</f>
+        <v>0.35673811186119631</v>
+      </c>
+    </row>
+    <row r="86" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>96</v>
+      </c>
+      <c r="B86" s="7">
+        <v>1.3971</v>
+      </c>
+      <c r="E86" s="5"/>
+      <c r="F86" s="5"/>
+      <c r="G86" s="5"/>
+      <c r="H86" s="5"/>
+      <c r="J86">
+        <f>0.0721*13</f>
+        <v>0.93730000000000002</v>
+      </c>
+      <c r="L86">
+        <f t="shared" si="19"/>
+        <v>-3.2844500000000001</v>
+      </c>
+      <c r="M86">
+        <f t="shared" si="20"/>
+        <v>-0.95005000000000006</v>
+      </c>
+      <c r="N86">
+        <f t="shared" si="21"/>
+        <v>0.38672168688674669</v>
+      </c>
+      <c r="O86">
+        <f t="shared" si="22"/>
+        <v>0.27887476668440547</v>
       </c>
     </row>
     <row r="87" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A87" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B87" t="s">
-        <v>4</v>
-      </c>
-      <c r="C87" t="s">
-        <v>73</v>
-      </c>
-      <c r="D87" t="s">
-        <v>6</v>
-      </c>
-      <c r="E87" t="s">
-        <v>64</v>
-      </c>
-      <c r="F87" t="s">
-        <v>7</v>
-      </c>
-      <c r="G87" t="s">
-        <v>8</v>
-      </c>
-      <c r="H87" t="s">
-        <v>35</v>
-      </c>
-      <c r="I87" t="s">
-        <v>29</v>
-      </c>
-      <c r="J87" t="s">
-        <v>36</v>
-      </c>
-      <c r="K87" t="s">
-        <v>11</v>
-      </c>
-      <c r="L87" t="s">
-        <v>54</v>
-      </c>
-      <c r="M87" t="s">
-        <v>12</v>
-      </c>
-      <c r="N87" t="s">
-        <v>13</v>
-      </c>
-      <c r="O87" t="s">
-        <v>14</v>
+      <c r="A87" t="s">
+        <v>97</v>
+      </c>
+      <c r="B87" s="7">
+        <v>1.3971</v>
+      </c>
+      <c r="D87" s="7">
+        <v>-9.1499999999999998E-2</v>
+      </c>
+      <c r="E87" s="5"/>
+      <c r="F87" s="5"/>
+      <c r="G87" s="5"/>
+      <c r="H87" s="5"/>
+      <c r="I87">
+        <f t="shared" ref="I87:I92" si="23">0.0721*18</f>
+        <v>1.2978000000000001</v>
+      </c>
+      <c r="L87">
+        <f t="shared" si="19"/>
+        <v>-3.2844500000000001</v>
+      </c>
+      <c r="M87">
+        <f t="shared" si="20"/>
+        <v>-0.68104999999999993</v>
+      </c>
+      <c r="N87">
+        <f t="shared" si="21"/>
+        <v>0.50608532369850301</v>
+      </c>
+      <c r="O87">
+        <f t="shared" si="22"/>
+        <v>0.33602699377994477</v>
       </c>
     </row>
     <row r="88" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>72</v>
-      </c>
-      <c r="B88" s="5">
-        <v>29.564</v>
-      </c>
+        <v>98</v>
+      </c>
+      <c r="B88" s="7">
+        <v>1.3971</v>
+      </c>
+      <c r="E88" s="7">
+        <v>-0.82440000000000002</v>
+      </c>
+      <c r="F88" s="5"/>
+      <c r="G88" s="5"/>
+      <c r="H88" s="5"/>
       <c r="I88">
-        <f>0.0424*18</f>
-        <v>0.76319999999999999</v>
+        <f t="shared" si="23"/>
+        <v>1.2978000000000001</v>
       </c>
       <c r="L88">
-        <f>-0.0154*2015</f>
-        <v>-31.031000000000002</v>
+        <f t="shared" si="19"/>
+        <v>-3.2844500000000001</v>
       </c>
       <c r="M88">
-        <f t="shared" ref="M88:M95" si="9">SUM(B88:L88)</f>
-        <v>-0.70380000000000109</v>
+        <f t="shared" si="20"/>
+        <v>-1.41395</v>
       </c>
       <c r="N88">
-        <f t="shared" ref="N88:N95" si="10">EXP(M88)</f>
-        <v>0.49470186044576797</v>
+        <f t="shared" si="21"/>
+        <v>0.2431808193024898</v>
       </c>
       <c r="O88">
-        <f t="shared" ref="O88:O95" si="11">N88/(N88+1)</f>
-        <v>0.33097025804077879</v>
+        <f t="shared" si="22"/>
+        <v>0.19561178512948021</v>
       </c>
     </row>
     <row r="89" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>80</v>
-      </c>
-      <c r="B89" s="5">
-        <v>29.564</v>
+        <v>99</v>
+      </c>
+      <c r="B89" s="7">
+        <v>1.3971</v>
       </c>
       <c r="E89" s="5"/>
-      <c r="F89" s="5"/>
+      <c r="F89" s="7">
+        <v>-0.68579999999999997</v>
+      </c>
       <c r="G89" s="5"/>
       <c r="H89" s="5"/>
-      <c r="J89">
-        <f>0.0424*13</f>
-        <v>0.55120000000000002</v>
+      <c r="I89">
+        <f t="shared" si="23"/>
+        <v>1.2978000000000001</v>
       </c>
       <c r="L89">
-        <f t="shared" ref="L89:L95" si="12">-0.0154*2015</f>
-        <v>-31.031000000000002</v>
+        <f t="shared" si="19"/>
+        <v>-3.2844500000000001</v>
       </c>
       <c r="M89">
-        <f t="shared" si="9"/>
-        <v>-0.91580000000000084</v>
+        <f t="shared" si="20"/>
+        <v>-1.27535</v>
       </c>
       <c r="N89">
-        <f t="shared" si="10"/>
-        <v>0.40019634092109557</v>
+        <f t="shared" si="21"/>
+        <v>0.27933318449568006</v>
       </c>
       <c r="O89">
-        <f t="shared" si="11"/>
-        <v>0.28581444560684477</v>
+        <f t="shared" si="22"/>
+        <v>0.21834279598226375</v>
       </c>
     </row>
     <row r="90" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>74</v>
-      </c>
-      <c r="B90" s="5">
-        <v>29.564</v>
-      </c>
-      <c r="D90">
-        <v>-2.76E-2</v>
+        <v>100</v>
+      </c>
+      <c r="B90" s="7">
+        <v>1.3971</v>
       </c>
       <c r="E90" s="5"/>
       <c r="F90" s="5"/>
       <c r="G90" s="5"/>
       <c r="H90" s="5"/>
       <c r="I90">
-        <f t="shared" ref="I90:I95" si="13">0.0424*18</f>
-        <v>0.76319999999999999</v>
-      </c>
-      <c r="L90">
-        <f t="shared" si="12"/>
-        <v>-31.031000000000002</v>
+        <f t="shared" si="23"/>
+        <v>1.2978000000000001</v>
+      </c>
+      <c r="K90">
+        <f>-0.00163*2014</f>
+        <v>-3.2828200000000001</v>
       </c>
       <c r="M90">
-        <f t="shared" si="9"/>
-        <v>-0.73140000000000072</v>
+        <f t="shared" si="20"/>
+        <v>-0.58792</v>
       </c>
       <c r="N90">
-        <f t="shared" si="10"/>
-        <v>0.48123478955457016</v>
+        <f t="shared" si="21"/>
+        <v>0.55548148543936005</v>
       </c>
       <c r="O90">
-        <f t="shared" si="11"/>
-        <v>0.32488758227133241</v>
+        <f t="shared" si="22"/>
+        <v>0.35711224507597344</v>
       </c>
     </row>
     <row r="91" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>79</v>
-      </c>
-      <c r="B91" s="5">
-        <v>29.564</v>
-      </c>
-      <c r="C91">
-        <v>-0.70169999999999999</v>
+        <v>101</v>
+      </c>
+      <c r="B91" s="7">
+        <v>1.3971</v>
       </c>
       <c r="E91" s="5"/>
       <c r="F91" s="5"/>
       <c r="G91" s="5"/>
-      <c r="H91" s="5"/>
+      <c r="H91" s="7">
+        <v>-8.2699999999999996E-3</v>
+      </c>
       <c r="I91">
-        <f t="shared" si="13"/>
-        <v>0.76319999999999999</v>
+        <f t="shared" si="23"/>
+        <v>1.2978000000000001</v>
       </c>
       <c r="L91">
-        <f t="shared" si="12"/>
-        <v>-31.031000000000002</v>
+        <f>-0.00163*2015</f>
+        <v>-3.2844500000000001</v>
       </c>
       <c r="M91">
-        <f t="shared" si="9"/>
-        <v>-1.4055</v>
+        <f t="shared" si="20"/>
+        <v>-0.59782000000000002</v>
       </c>
       <c r="N91">
-        <f t="shared" si="10"/>
-        <v>0.24524440359047078</v>
+        <f t="shared" si="21"/>
+        <v>0.55000935049507371</v>
       </c>
       <c r="O91">
-        <f t="shared" si="11"/>
-        <v>0.19694479483974892</v>
+        <f t="shared" si="22"/>
+        <v>0.35484260163940334</v>
       </c>
     </row>
     <row r="92" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>75</v>
-      </c>
-      <c r="B92" s="5">
-        <v>29.564</v>
-      </c>
-      <c r="E92" s="5">
-        <v>-0.2082</v>
-      </c>
+        <v>94</v>
+      </c>
+      <c r="B92" s="7">
+        <v>1.3971</v>
+      </c>
+      <c r="C92" s="7">
+        <v>0.18229999999999999</v>
+      </c>
+      <c r="E92" s="5"/>
       <c r="F92" s="5"/>
       <c r="G92" s="5"/>
       <c r="H92" s="5"/>
       <c r="I92">
-        <f t="shared" si="13"/>
-        <v>0.76319999999999999</v>
+        <f t="shared" si="23"/>
+        <v>1.2978000000000001</v>
       </c>
       <c r="L92">
-        <f t="shared" si="12"/>
-        <v>-31.031000000000002</v>
+        <f>-0.00163*2015</f>
+        <v>-3.2844500000000001</v>
       </c>
       <c r="M92">
-        <f t="shared" si="9"/>
-        <v>-0.91200000000000259</v>
+        <f t="shared" si="20"/>
+        <v>-0.40724999999999989</v>
       </c>
       <c r="N92">
-        <f t="shared" si="10"/>
-        <v>0.40171998009758503</v>
+        <f>EXP(M92)</f>
+        <v>0.66547780005359358</v>
       </c>
       <c r="O92">
-        <f t="shared" si="11"/>
-        <v>0.28659074979413368</v>
-      </c>
-    </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
-        <v>76</v>
-      </c>
-      <c r="B93" s="5">
-        <v>29.564</v>
-      </c>
-      <c r="E93" s="5"/>
-      <c r="F93" s="5">
-        <v>-0.43090000000000001</v>
-      </c>
-      <c r="G93" s="5"/>
-      <c r="H93" s="5"/>
-      <c r="I93">
-        <f t="shared" si="13"/>
-        <v>0.76319999999999999</v>
-      </c>
-      <c r="L93">
-        <f t="shared" si="12"/>
-        <v>-31.031000000000002</v>
-      </c>
-      <c r="M93">
-        <f t="shared" si="9"/>
-        <v>-1.1347000000000023</v>
-      </c>
-      <c r="N93">
-        <f t="shared" si="10"/>
-        <v>0.32151856243623289</v>
-      </c>
-      <c r="O93">
-        <f t="shared" si="11"/>
-        <v>0.24329477585506643</v>
-      </c>
-    </row>
-    <row r="94" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
-        <v>77</v>
-      </c>
-      <c r="B94" s="5">
-        <v>29.564</v>
-      </c>
-      <c r="E94" s="5"/>
-      <c r="F94" s="5"/>
-      <c r="G94" s="5"/>
-      <c r="H94" s="5"/>
-      <c r="I94">
-        <f t="shared" si="13"/>
-        <v>0.76319999999999999</v>
-      </c>
-      <c r="K94">
-        <f>-0.0154*2014</f>
-        <v>-31.015600000000003</v>
-      </c>
-      <c r="M94">
-        <f t="shared" si="9"/>
-        <v>-0.68840000000000146</v>
-      </c>
-      <c r="N94">
-        <f t="shared" si="10"/>
-        <v>0.50237923313647515</v>
-      </c>
-      <c r="O94">
-        <f t="shared" si="11"/>
-        <v>0.33438909567970537</v>
-      </c>
-    </row>
-    <row r="95" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
-        <v>78</v>
-      </c>
-      <c r="B95" s="5">
-        <v>29.564</v>
-      </c>
-      <c r="E95" s="5"/>
-      <c r="F95" s="5"/>
-      <c r="G95" s="5"/>
-      <c r="H95" s="5">
-        <v>-1.4E-2</v>
-      </c>
-      <c r="I95">
-        <f t="shared" si="13"/>
-        <v>0.76319999999999999</v>
-      </c>
-      <c r="L95">
-        <f t="shared" si="12"/>
-        <v>-31.031000000000002</v>
-      </c>
-      <c r="M95">
-        <f t="shared" si="9"/>
-        <v>-0.71780000000000044</v>
-      </c>
-      <c r="N95">
-        <f t="shared" si="10"/>
-        <v>0.48782428972784109</v>
-      </c>
-      <c r="O95">
-        <f t="shared" si="11"/>
-        <v>0.32787762177015939</v>
-      </c>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A97" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+        <f>N92/(N92+1)</f>
+        <v>0.3995717025061391</v>
+      </c>
+    </row>
+    <row r="96" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A96" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B96" t="s">
+        <v>4</v>
+      </c>
+      <c r="C96" t="s">
+        <v>111</v>
+      </c>
+      <c r="D96" t="s">
+        <v>6</v>
+      </c>
+      <c r="E96" t="s">
+        <v>62</v>
+      </c>
+      <c r="F96" t="s">
+        <v>7</v>
+      </c>
+      <c r="G96" t="s">
+        <v>8</v>
+      </c>
+      <c r="H96" t="s">
+        <v>33</v>
+      </c>
+      <c r="I96" t="s">
+        <v>29</v>
+      </c>
+      <c r="J96" t="s">
+        <v>34</v>
+      </c>
+      <c r="K96" t="s">
+        <v>11</v>
+      </c>
+      <c r="L96" t="s">
+        <v>52</v>
+      </c>
+      <c r="M96" t="s">
+        <v>12</v>
+      </c>
+      <c r="N96" t="s">
+        <v>13</v>
+      </c>
+      <c r="O96" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="97" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>103</v>
+      </c>
+      <c r="B97" s="7">
+        <v>-5.9520999999999997</v>
+      </c>
+      <c r="I97">
+        <f>0.00347*18</f>
+        <v>6.2460000000000002E-2</v>
+      </c>
+      <c r="L97">
+        <f>0.00281*2015</f>
+        <v>5.6621499999999996</v>
+      </c>
+      <c r="M97">
+        <f t="shared" ref="M97:M104" si="24">SUM(B97:L97)</f>
+        <v>-0.22749000000000041</v>
+      </c>
+      <c r="N97">
+        <f t="shared" ref="N97:N103" si="25">EXP(M97)</f>
+        <v>0.79653038676153287</v>
+      </c>
+      <c r="O97">
+        <f t="shared" ref="O97:O103" si="26">N97/(N97+1)</f>
+        <v>0.44337150800848796</v>
+      </c>
+    </row>
+    <row r="98" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+      <c r="B98" s="7">
+        <v>-5.9520999999999997</v>
+      </c>
+      <c r="E98" s="5"/>
+      <c r="F98" s="5"/>
+      <c r="G98" s="5"/>
+      <c r="H98" s="5"/>
+      <c r="J98">
+        <f>0.00347*13</f>
+        <v>4.5109999999999997E-2</v>
+      </c>
+      <c r="L98">
+        <f t="shared" ref="L98:L104" si="27">0.00281*2015</f>
+        <v>5.6621499999999996</v>
+      </c>
+      <c r="M98">
+        <f t="shared" si="24"/>
+        <v>-0.24483999999999995</v>
+      </c>
+      <c r="N98">
+        <f t="shared" si="25"/>
+        <v>0.7828297809871394</v>
+      </c>
+      <c r="O98">
+        <f t="shared" si="26"/>
+        <v>0.43909395576379279</v>
+      </c>
+    </row>
+    <row r="99" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+      <c r="B99" s="7">
+        <v>-5.9520999999999997</v>
+      </c>
+      <c r="D99" s="8">
+        <v>-0.11459999999999999</v>
+      </c>
+      <c r="E99" s="5"/>
+      <c r="F99" s="5"/>
+      <c r="G99" s="5"/>
+      <c r="H99" s="5"/>
+      <c r="I99">
+        <f t="shared" ref="I98:J104" si="28">0.00347*18</f>
+        <v>6.2460000000000002E-2</v>
+      </c>
+      <c r="L99">
+        <f t="shared" si="27"/>
+        <v>5.6621499999999996</v>
+      </c>
+      <c r="M99">
+        <f t="shared" si="24"/>
+        <v>-0.34209000000000067</v>
+      </c>
+      <c r="N99">
+        <f t="shared" si="25"/>
+        <v>0.71028427624757684</v>
+      </c>
+      <c r="O99">
+        <f t="shared" si="26"/>
+        <v>0.41530188057740036</v>
+      </c>
+    </row>
+    <row r="100" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+      <c r="B100" s="7">
+        <v>-5.9520999999999997</v>
+      </c>
+      <c r="E100" s="8">
+        <v>-1.1100000000000001</v>
+      </c>
+      <c r="F100" s="5"/>
+      <c r="G100" s="5"/>
+      <c r="H100" s="5"/>
+      <c r="I100">
+        <f t="shared" si="28"/>
+        <v>6.2460000000000002E-2</v>
+      </c>
+      <c r="L100">
+        <f t="shared" si="27"/>
+        <v>5.6621499999999996</v>
+      </c>
+      <c r="M100">
+        <f t="shared" si="24"/>
+        <v>-1.3374900000000007</v>
+      </c>
+      <c r="N100">
+        <f t="shared" si="25"/>
+        <v>0.26250372672594918</v>
+      </c>
+      <c r="O100">
+        <f t="shared" si="26"/>
+        <v>0.20792313018093031</v>
+      </c>
+    </row>
+    <row r="101" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A114" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A115" t="s">
-        <v>85</v>
+        <v>107</v>
+      </c>
+      <c r="B101" s="7">
+        <v>-5.9520999999999997</v>
+      </c>
+      <c r="E101" s="5"/>
+      <c r="F101" s="8">
+        <v>-0.34189999999999998</v>
+      </c>
+      <c r="G101" s="5"/>
+      <c r="H101" s="5"/>
+      <c r="I101">
+        <f t="shared" si="28"/>
+        <v>6.2460000000000002E-2</v>
+      </c>
+      <c r="L101">
+        <f t="shared" si="27"/>
+        <v>5.6621499999999996</v>
+      </c>
+      <c r="M101">
+        <f t="shared" si="24"/>
+        <v>-0.56939000000000028</v>
+      </c>
+      <c r="N101">
+        <f t="shared" si="25"/>
+        <v>0.56587051445454872</v>
+      </c>
+      <c r="O101">
+        <f t="shared" si="26"/>
+        <v>0.36137759107857181</v>
+      </c>
+    </row>
+    <row r="102" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>108</v>
+      </c>
+      <c r="B102" s="7">
+        <v>-5.9520999999999997</v>
+      </c>
+      <c r="E102" s="5"/>
+      <c r="F102" s="5"/>
+      <c r="G102" s="5"/>
+      <c r="H102" s="5"/>
+      <c r="I102">
+        <f t="shared" si="28"/>
+        <v>6.2460000000000002E-2</v>
+      </c>
+      <c r="K102">
+        <f>0.00281*2014</f>
+        <v>5.6593400000000003</v>
+      </c>
+      <c r="M102">
+        <f t="shared" si="24"/>
+        <v>-0.23029999999999973</v>
+      </c>
+      <c r="N102">
+        <f t="shared" si="25"/>
+        <v>0.79429527817302026</v>
+      </c>
+      <c r="O102">
+        <f t="shared" si="26"/>
+        <v>0.44267812986822563</v>
+      </c>
+    </row>
+    <row r="103" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>109</v>
+      </c>
+      <c r="B103" s="7">
+        <v>-5.9520999999999997</v>
+      </c>
+      <c r="E103" s="5"/>
+      <c r="F103" s="5"/>
+      <c r="G103" s="5"/>
+      <c r="H103" s="8">
+        <v>4.0300000000000002E-2</v>
+      </c>
+      <c r="I103">
+        <f t="shared" si="28"/>
+        <v>6.2460000000000002E-2</v>
+      </c>
+      <c r="L103">
+        <f t="shared" si="27"/>
+        <v>5.6621499999999996</v>
+      </c>
+      <c r="M103">
+        <f t="shared" si="24"/>
+        <v>-0.18719000000000019</v>
+      </c>
+      <c r="N103">
+        <f t="shared" si="25"/>
+        <v>0.82928615704600184</v>
+      </c>
+      <c r="O103">
+        <f t="shared" si="26"/>
+        <v>0.45333867194685573</v>
+      </c>
+    </row>
+    <row r="104" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>110</v>
+      </c>
+      <c r="B104" s="7">
+        <v>-5.9520999999999997</v>
+      </c>
+      <c r="C104" s="8">
+        <v>-0.1973</v>
+      </c>
+      <c r="E104" s="5"/>
+      <c r="F104" s="5"/>
+      <c r="G104" s="5"/>
+      <c r="H104" s="5"/>
+      <c r="I104">
+        <f t="shared" si="28"/>
+        <v>6.2460000000000002E-2</v>
+      </c>
+      <c r="L104">
+        <f t="shared" si="27"/>
+        <v>5.6621499999999996</v>
+      </c>
+      <c r="M104">
+        <f t="shared" si="24"/>
+        <v>-0.42479000000000067</v>
+      </c>
+      <c r="N104">
+        <f>EXP(M104)</f>
+        <v>0.65390709120135704</v>
+      </c>
+      <c r="O104">
+        <f>N104/(N104+1)</f>
+        <v>0.39537111527006952</v>
       </c>
     </row>
   </sheetData>
@@ -2323,122 +3426,200 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C2" t="s">
         <v>30</v>
       </c>
       <c r="D2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" t="s">
         <v>42</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>43</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>44</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
         <v>45</v>
-      </c>
-      <c r="H2" t="s">
-        <v>46</v>
-      </c>
-      <c r="I2" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B3" t="s">
-        <v>60</v>
+        <v>58</v>
+      </c>
+      <c r="C3" t="s">
+        <v>58</v>
       </c>
       <c r="D3" t="s">
-        <v>60</v>
+        <v>58</v>
+      </c>
+      <c r="E3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F3" t="s">
+        <v>58</v>
+      </c>
+      <c r="H3" t="s">
+        <v>58</v>
       </c>
       <c r="I3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B4" t="s">
-        <v>60</v>
+        <v>58</v>
+      </c>
+      <c r="C4" t="s">
+        <v>58</v>
       </c>
       <c r="D4" t="s">
-        <v>60</v>
+        <v>58</v>
+      </c>
+      <c r="E4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F4" t="s">
+        <v>58</v>
+      </c>
+      <c r="H4" t="s">
+        <v>58</v>
       </c>
       <c r="I4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B5" t="s">
-        <v>60</v>
+        <v>58</v>
+      </c>
+      <c r="C5" t="s">
+        <v>58</v>
       </c>
       <c r="D5" t="s">
-        <v>60</v>
+        <v>58</v>
+      </c>
+      <c r="E5" t="s">
+        <v>58</v>
+      </c>
+      <c r="F5" t="s">
+        <v>58</v>
+      </c>
+      <c r="G5" t="s">
+        <v>58</v>
+      </c>
+      <c r="H5" t="s">
+        <v>58</v>
       </c>
       <c r="I5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B6" t="s">
-        <v>60</v>
+        <v>58</v>
+      </c>
+      <c r="C6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E6" t="s">
+        <v>58</v>
+      </c>
+      <c r="F6" t="s">
+        <v>58</v>
+      </c>
+      <c r="H6" t="s">
+        <v>58</v>
       </c>
       <c r="I6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B7" t="s">
-        <v>60</v>
+        <v>58</v>
+      </c>
+      <c r="C7" t="s">
+        <v>58</v>
+      </c>
+      <c r="E7" t="s">
+        <v>58</v>
+      </c>
+      <c r="F7" t="s">
+        <v>58</v>
+      </c>
+      <c r="H7" t="s">
+        <v>58</v>
       </c>
       <c r="I7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B8" t="s">
-        <v>60</v>
+        <v>58</v>
+      </c>
+      <c r="C8" t="s">
+        <v>58</v>
       </c>
       <c r="D8" t="s">
-        <v>60</v>
+        <v>58</v>
+      </c>
+      <c r="E8" t="s">
+        <v>58</v>
+      </c>
+      <c r="F8" t="s">
+        <v>58</v>
+      </c>
+      <c r="G8" t="s">
+        <v>58</v>
+      </c>
+      <c r="H8" t="s">
+        <v>58</v>
       </c>
       <c r="I8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -2446,10 +3627,22 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>60</v>
+        <v>58</v>
+      </c>
+      <c r="C9" t="s">
+        <v>58</v>
+      </c>
+      <c r="E9" t="s">
+        <v>58</v>
+      </c>
+      <c r="F9" t="s">
+        <v>58</v>
+      </c>
+      <c r="H9" t="s">
+        <v>58</v>
       </c>
       <c r="I9" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>